<commit_message>
Change to "Transport not elsewhere specified"
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample-2021.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample-2021.xlsx
@@ -380,9 +380,6 @@
     <t>Pipeline transport</t>
   </si>
   <si>
-    <t>Non-specified (transport)</t>
-  </si>
-  <si>
     <t>Coal stoves</t>
   </si>
   <si>
@@ -408,6 +405,9 @@
   </si>
   <si>
     <t>Paraffin waxes</t>
+  </si>
+  <si>
+    <t>Transport not elsewhere specified</t>
   </si>
 </sst>
 </file>
@@ -869,8 +869,8 @@
   <dimension ref="A1:O759"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K173" sqref="K173"/>
+      <pane ySplit="1" topLeftCell="A529" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K557" sqref="K557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22604,7 +22604,7 @@
       <c r="I543" s="7"/>
       <c r="J543" s="7"/>
       <c r="K543" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L543" s="7" t="s">
         <v>24</v>
@@ -22645,7 +22645,7 @@
       <c r="I544" s="7"/>
       <c r="J544" s="7"/>
       <c r="K544" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L544" s="7" t="s">
         <v>25</v>
@@ -22690,7 +22690,7 @@
         <v>43</v>
       </c>
       <c r="K545" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L545" t="s">
         <v>28</v>
@@ -22727,7 +22727,7 @@
         <v>44</v>
       </c>
       <c r="K546" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L546" t="s">
         <v>29</v>
@@ -22762,7 +22762,7 @@
         <v>44</v>
       </c>
       <c r="K547" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L547" t="s">
         <v>30</v>
@@ -22799,7 +22799,7 @@
       <c r="I548" s="7"/>
       <c r="J548" s="7"/>
       <c r="K548" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L548" s="7" t="s">
         <v>24</v>
@@ -22840,7 +22840,7 @@
       <c r="I549" s="7"/>
       <c r="J549" s="7"/>
       <c r="K549" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L549" s="7" t="s">
         <v>25</v>
@@ -22885,7 +22885,7 @@
         <v>34</v>
       </c>
       <c r="K550" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L550" t="s">
         <v>28</v>
@@ -22928,7 +22928,7 @@
         <v>43</v>
       </c>
       <c r="K551" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L551" t="s">
         <v>29</v>
@@ -22965,7 +22965,7 @@
         <v>46</v>
       </c>
       <c r="K552" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L552" t="s">
         <v>30</v>
@@ -23002,7 +23002,7 @@
       <c r="I553" s="7"/>
       <c r="J553" s="7"/>
       <c r="K553" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L553" s="7" t="s">
         <v>24</v>
@@ -23045,7 +23045,7 @@
       <c r="I554" s="7"/>
       <c r="J554" s="7"/>
       <c r="K554" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L554" s="7" t="s">
         <v>25</v>
@@ -23092,7 +23092,7 @@
         <v>36</v>
       </c>
       <c r="K555" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L555" t="s">
         <v>28</v>
@@ -23131,7 +23131,7 @@
         <v>31</v>
       </c>
       <c r="K556" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L556" t="s">
         <v>29</v>
@@ -23166,7 +23166,7 @@
         <v>31</v>
       </c>
       <c r="K557" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L557" t="s">
         <v>30</v>
@@ -23283,10 +23283,10 @@
         <v>92</v>
       </c>
       <c r="I560" t="s">
+        <v>118</v>
+      </c>
+      <c r="J560" t="s">
         <v>119</v>
-      </c>
-      <c r="J560" t="s">
-        <v>120</v>
       </c>
       <c r="K560" t="s">
         <v>62</v>
@@ -23478,10 +23478,10 @@
         <v>93</v>
       </c>
       <c r="I565" t="s">
+        <v>118</v>
+      </c>
+      <c r="J565" t="s">
         <v>119</v>
-      </c>
-      <c r="J565" t="s">
-        <v>120</v>
       </c>
       <c r="K565" t="s">
         <v>62</v>
@@ -23877,7 +23877,7 @@
         <v>63</v>
       </c>
       <c r="J575" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K575" t="s">
         <v>62</v>
@@ -23917,7 +23917,7 @@
         <v>44</v>
       </c>
       <c r="I576" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J576" t="s">
         <v>64</v>
@@ -24077,7 +24077,7 @@
         <v>52</v>
       </c>
       <c r="I580" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J580" t="s">
         <v>36</v>
@@ -24275,7 +24275,7 @@
         <v>65</v>
       </c>
       <c r="J585" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K585" t="s">
         <v>62</v>
@@ -24470,7 +24470,7 @@
         <v>103</v>
       </c>
       <c r="J590" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K590" t="s">
         <v>62</v>
@@ -24665,7 +24665,7 @@
         <v>103</v>
       </c>
       <c r="J595" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K595" t="s">
         <v>62</v>
@@ -24906,10 +24906,10 @@
         <v>49</v>
       </c>
       <c r="I601" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J601" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K601" t="s">
         <v>62</v>
@@ -25490,10 +25490,10 @@
         <v>92</v>
       </c>
       <c r="I615" t="s">
+        <v>118</v>
+      </c>
+      <c r="J615" t="s">
         <v>119</v>
-      </c>
-      <c r="J615" t="s">
-        <v>120</v>
       </c>
       <c r="K615" t="s">
         <v>73</v>
@@ -25685,10 +25685,10 @@
         <v>93</v>
       </c>
       <c r="I620" t="s">
+        <v>118</v>
+      </c>
+      <c r="J620" t="s">
         <v>119</v>
-      </c>
-      <c r="J620" t="s">
-        <v>120</v>
       </c>
       <c r="K620" t="s">
         <v>73</v>
@@ -26861,10 +26861,10 @@
         <v>48</v>
       </c>
       <c r="I650" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J650" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K650" t="s">
         <v>73</v>
@@ -27267,7 +27267,7 @@
         <v>92</v>
       </c>
       <c r="I660" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J660" t="s">
         <v>43</v>
@@ -27462,7 +27462,7 @@
         <v>93</v>
       </c>
       <c r="I665" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J665" t="s">
         <v>64</v>
@@ -28058,7 +28058,7 @@
         <v>65</v>
       </c>
       <c r="J680" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K680" t="s">
         <v>74</v>
@@ -28257,7 +28257,7 @@
         <v>103</v>
       </c>
       <c r="J685" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K685" t="s">
         <v>74</v>
@@ -28451,7 +28451,7 @@
         <v>48</v>
       </c>
       <c r="I690" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J690" t="s">
         <v>43</v>
@@ -29159,7 +29159,7 @@
       <c r="I708" s="7"/>
       <c r="J708" s="7"/>
       <c r="K708" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L708" s="7" t="s">
         <v>24</v>
@@ -29200,7 +29200,7 @@
       <c r="I709" s="7"/>
       <c r="J709" s="7"/>
       <c r="K709" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L709" s="7" t="s">
         <v>25</v>
@@ -29245,7 +29245,7 @@
         <v>43</v>
       </c>
       <c r="K710" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L710" t="s">
         <v>28</v>
@@ -29282,7 +29282,7 @@
         <v>44</v>
       </c>
       <c r="K711" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L711" t="s">
         <v>29</v>
@@ -29317,7 +29317,7 @@
         <v>44</v>
       </c>
       <c r="K712" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L712" t="s">
         <v>30</v>
@@ -29354,7 +29354,7 @@
       <c r="I713" s="7"/>
       <c r="J713" s="7"/>
       <c r="K713" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L713" s="7" t="s">
         <v>24</v>
@@ -29397,7 +29397,7 @@
       <c r="I714" s="7"/>
       <c r="J714" s="7"/>
       <c r="K714" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L714" s="7" t="s">
         <v>25</v>
@@ -29444,7 +29444,7 @@
         <v>43</v>
       </c>
       <c r="K715" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L715" t="s">
         <v>28</v>
@@ -29483,7 +29483,7 @@
         <v>46</v>
       </c>
       <c r="K716" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L716" t="s">
         <v>29</v>
@@ -29518,7 +29518,7 @@
         <v>46</v>
       </c>
       <c r="K717" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L717" t="s">
         <v>30</v>
@@ -29555,7 +29555,7 @@
       <c r="I718" s="7"/>
       <c r="J718" s="7"/>
       <c r="K718" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L718" s="7" t="s">
         <v>24</v>
@@ -29596,7 +29596,7 @@
       <c r="I719" s="7"/>
       <c r="J719" s="7"/>
       <c r="K719" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L719" s="7" t="s">
         <v>25</v>
@@ -29641,7 +29641,7 @@
         <v>43</v>
       </c>
       <c r="K720" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L720" t="s">
         <v>28</v>
@@ -29678,7 +29678,7 @@
         <v>47</v>
       </c>
       <c r="K721" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L721" t="s">
         <v>29</v>
@@ -29713,7 +29713,7 @@
         <v>47</v>
       </c>
       <c r="K722" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L722" t="s">
         <v>30</v>
@@ -29750,7 +29750,7 @@
       <c r="I723" s="7"/>
       <c r="J723" s="7"/>
       <c r="K723" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L723" s="7" t="s">
         <v>24</v>
@@ -29793,7 +29793,7 @@
       <c r="I724" s="7"/>
       <c r="J724" s="7"/>
       <c r="K724" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L724" s="7" t="s">
         <v>25</v>
@@ -29840,7 +29840,7 @@
         <v>34</v>
       </c>
       <c r="K725" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L725" t="s">
         <v>28</v>
@@ -29885,7 +29885,7 @@
         <v>36</v>
       </c>
       <c r="K726" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L726" t="s">
         <v>29</v>
@@ -29924,7 +29924,7 @@
         <v>31</v>
       </c>
       <c r="K727" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L727" t="s">
         <v>30</v>
@@ -29959,7 +29959,7 @@
         <v>31</v>
       </c>
       <c r="K728" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L728" t="s">
         <v>72</v>
@@ -30381,7 +30381,7 @@
         <v>21</v>
       </c>
       <c r="H739" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I739" s="10"/>
       <c r="J739" s="10"/>
@@ -30422,7 +30422,7 @@
         <v>21</v>
       </c>
       <c r="H740" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I740" s="10"/>
       <c r="J740" s="10"/>
@@ -30463,13 +30463,13 @@
         <v>21</v>
       </c>
       <c r="H741" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I741" t="s">
         <v>80</v>
       </c>
       <c r="J741" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K741" t="s">
         <v>79</v>
@@ -30506,7 +30506,7 @@
         <v>21</v>
       </c>
       <c r="H742" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K742" t="s">
         <v>79</v>
@@ -30541,7 +30541,7 @@
         <v>21</v>
       </c>
       <c r="H743" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K743" t="s">
         <v>79</v>
@@ -30972,7 +30972,7 @@
         <v>21</v>
       </c>
       <c r="H754" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I754" s="10"/>
       <c r="J754" s="10"/>
@@ -31013,7 +31013,7 @@
         <v>21</v>
       </c>
       <c r="H755" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I755" s="10"/>
       <c r="J755" s="10"/>
@@ -31054,13 +31054,13 @@
         <v>21</v>
       </c>
       <c r="H756" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I756" t="s">
         <v>80</v>
       </c>
       <c r="J756" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K756" t="s">
         <v>79</v>
@@ -31097,7 +31097,7 @@
         <v>21</v>
       </c>
       <c r="H757" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K757" t="s">
         <v>79</v>
@@ -31132,7 +31132,7 @@
         <v>21</v>
       </c>
       <c r="H758" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K758" t="s">
         <v>79</v>
@@ -31167,7 +31167,7 @@
         <v>21</v>
       </c>
       <c r="H759" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K759" t="s">
         <v>79</v>

</xml_diff>